<commit_message>
[AGR] Add Wolf species template
</commit_message>
<xml_diff>
--- a/Agranari/Species_Templates.xlsx
+++ b/Agranari/Species_Templates.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Stories\DnD-Stories\Agranari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B25C89-028E-458B-925C-AD81B69255D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72953C2-1216-4360-85BE-D61E14A1A925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{6B096DA7-CFA8-4C5C-A879-5A8B21184BB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Deer" sheetId="2" r:id="rId1"/>
-    <sheet name="Bear" sheetId="1" r:id="rId2"/>
+    <sheet name="Wolf" sheetId="3" r:id="rId1"/>
+    <sheet name="Deer" sheetId="2" r:id="rId2"/>
+    <sheet name="Bear" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="95">
   <si>
     <t>BloodlustMaxRange</t>
   </si>
@@ -172,6 +173,156 @@
   </si>
   <si>
     <t>1d20</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>HighSightPower</t>
+  </si>
+  <si>
+    <t>1d10 (Disadv x2)</t>
+  </si>
+  <si>
+    <t>HindSightUnit</t>
+  </si>
+  <si>
+    <t>1d10 (Disadv x3)</t>
+  </si>
+  <si>
+    <t>HindSightMaxRewind</t>
+  </si>
+  <si>
+    <t>1d100 (Disadv x2)</t>
+  </si>
+  <si>
+    <t>RewindsThisHindSight</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>HindSightRewindSpeed</t>
+  </si>
+  <si>
+    <t>ForwardsThisHindSight</t>
+  </si>
+  <si>
+    <t>HindSightForwardSpeed</t>
+  </si>
+  <si>
+    <t>1d100 (Disadv)</t>
+  </si>
+  <si>
+    <t>HindSightTrackHead</t>
+  </si>
+  <si>
+    <t>AdrenalinePower</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>AdrenalineDuration</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>AdrenalineACBonus</t>
+  </si>
+  <si>
+    <t>AC bonus</t>
+  </si>
+  <si>
+    <t>Base AC</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AdrenalineToHitBonus</t>
+  </si>
+  <si>
+    <t>atk bonus</t>
+  </si>
+  <si>
+    <t>Bonus AC</t>
+  </si>
+  <si>
+    <t>AdrenalineMovementBonus</t>
+  </si>
+  <si>
+    <t>Total General AC</t>
+  </si>
+  <si>
+    <t>JumpACBonus</t>
+  </si>
+  <si>
+    <t>AdrenalineCharges</t>
+  </si>
+  <si>
+    <t>2d4</t>
+  </si>
+  <si>
+    <t>charges</t>
+  </si>
+  <si>
+    <t>Adrenaline Rush duration</t>
+  </si>
+  <si>
+    <t>EnemyCCSaveBonus</t>
+  </si>
+  <si>
+    <t>1d10 (Ax1, Dx1)</t>
+  </si>
+  <si>
+    <t>DEX save bonus</t>
+  </si>
+  <si>
+    <t>Exhaustion gained</t>
+  </si>
+  <si>
+    <t>exhaustion</t>
+  </si>
+  <si>
+    <t>TrackPreyMinTime</t>
+  </si>
+  <si>
+    <t>TrackPreyCritRange</t>
+  </si>
+  <si>
+    <t>crit range</t>
+  </si>
+  <si>
+    <t>TrackPreyToHitBonus</t>
+  </si>
+  <si>
+    <t>ProneEnemyACBonus</t>
+  </si>
+  <si>
+    <t>1d10 (Adv)</t>
+  </si>
+  <si>
+    <t>LickWoundsHeal</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>Opponent</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Crit</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Dodge</t>
   </si>
 </sst>
 </file>
@@ -213,7 +364,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -245,12 +396,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -267,6 +455,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +772,510 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F6C442-DD69-4ACA-B2EF-5810317D8DB0}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="12">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f>C5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" t="str">
+        <f>IF(C6=1,"Seconds",IF(C6=2,"Minutes",IF(C6=3,"Hours",IF(C6=4,"Days",IF(C6=5,"Weeks",IF(C6=6,"Months",IF(C6=7,"Years",IF(C6=8,"Decades",IF(C6=9,"Centuries",IF(C6=10,"Millenia","INVALID"))))))))))</f>
+        <v>Weeks</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="13">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <f>C7</f>
+        <v>8</v>
+      </c>
+      <c r="E7" t="str">
+        <f>E6</f>
+        <v>Weeks</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="2">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <f>D7*C8/100</f>
+        <v>1.52</v>
+      </c>
+      <c r="E8" t="str">
+        <f>E6</f>
+        <v>Weeks</v>
+      </c>
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="2">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <f>D7*C9/100</f>
+        <v>3.2</v>
+      </c>
+      <c r="E9" t="str">
+        <f>E6</f>
+        <v>Weeks</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="6">
+        <f>MIN(0,MAX(-D7,-(H7*D8)+(H8*D9)))</f>
+        <v>0</v>
+      </c>
+      <c r="K9" t="str">
+        <f>E6</f>
+        <v>Weeks</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <f>C6</f>
+        <v>5</v>
+      </c>
+      <c r="J10" s="6">
+        <f>J9*7</f>
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f>C11+D10</f>
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="6">
+        <f>J10/30</f>
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f>ROUNDUP(C12+D10/2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="2">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="14">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f>ROUNDUP(C13+D10/2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="2">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f>ROUNDUP((D4*C14*D10/75)/5,0)*5</f>
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14">
+        <f>H12+H13</f>
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <f>C15</f>
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <f>C16</f>
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="2">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="2">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <f>C17</f>
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17">
+        <f>ROUNDUP(ROUNDDOWN(H16/(D11/2),0)*(D11/2)/D11,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="14">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <f>11-C18</f>
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <f>C20</f>
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="2">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <f>C21</f>
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <f>ROUNDUP(C22/2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE37CB70-2D27-4892-9A0E-2EB7AE2FAFFD}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -826,7 +1517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54198961-A6A3-46E4-9FB5-2E30BF5550C8}">
   <dimension ref="A2:I12"/>
   <sheetViews>

</xml_diff>